<commit_message>
update dates of notes report
</commit_message>
<xml_diff>
--- a/docs/_static/FormatoPlaneacionInteractivos12023-10.xlsx
+++ b/docs/_static/FormatoPlaneacionInteractivos12023-10.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4620F03E-6C57-428A-BD1C-76B20A19AB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76988EA2-D9F0-464B-B1D6-481B7BCAB805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
   <si>
     <t>PROYECTO DOCENTE</t>
   </si>
@@ -327,56 +327,65 @@
     <t>Sitio web del curso versión 2022-20 https://sistemasfisicosinteractivos1.readthedocs.io/es/v2022.20/</t>
   </si>
   <si>
-    <t>Introducción al curso</t>
-  </si>
-  <si>
     <t>1 h 40 min. Presentación del curso</t>
   </si>
   <si>
-    <t xml:space="preserve">1 h 40 minutos Taller de control de versión </t>
-  </si>
-  <si>
-    <t>2 h. Realizar el material sobre control de versión</t>
-  </si>
-  <si>
     <t>https://sistemasfisicosinteractivos1.readthedocs.io/</t>
   </si>
   <si>
-    <t>Software para sistemas embebidos</t>
-  </si>
-  <si>
-    <t>3 h 20 min. Ejercicios de la unidad en el sitio web</t>
-  </si>
-  <si>
-    <t>3h 20 min. Solución a la evaluación y sustentación</t>
-  </si>
-  <si>
-    <t>2 h. Solución a la evaluación</t>
-  </si>
-  <si>
-    <t>2 h. Revisión del material del sitio web</t>
-  </si>
-  <si>
     <t>Formativa</t>
   </si>
   <si>
     <t>Sumativa</t>
   </si>
   <si>
-    <t>Protocolos ASCII</t>
-  </si>
-  <si>
-    <t>Protocolos binarios</t>
-  </si>
-  <si>
-    <t>Plataformas de software interactivas de tiempo real</t>
+    <t>2 h. Evaluación sobre control de versión</t>
+  </si>
+  <si>
+    <t>1 h 40 min. Terminar la evaluación y asesorías</t>
+  </si>
+  <si>
+    <t>Introducción al curso y evaluación sumativa sobre control de versión para la entrega de evaluaciones</t>
+  </si>
+  <si>
+    <t>2 h. Realización de los ejercicios de la unidad</t>
+  </si>
+  <si>
+    <t>3 h 20 min. Realizar los ejercicios de la unidad y asesorías</t>
+  </si>
+  <si>
+    <t>Unidad 1: software para sistemas embebidos</t>
+  </si>
+  <si>
+    <t>2 h. Terminar los ejercicios de la unidad</t>
+  </si>
+  <si>
+    <t>2 h. Trabajar en la solución de la evaluación de la unidad</t>
+  </si>
+  <si>
+    <t>3 h 20 min. Trabajar en la solución de la evaluación de la unidad</t>
+  </si>
+  <si>
+    <t>2 h. Montaje en el portafolio de los resultados de la evaluación</t>
+  </si>
+  <si>
+    <t>1 h 40 min. Sustentación y presentación del portafolio</t>
+  </si>
+  <si>
+    <t>Unidad 2: protocolos ASCII</t>
+  </si>
+  <si>
+    <t>Unidad 3: protocolos binarios</t>
+  </si>
+  <si>
+    <t>Unidad 4: plataformas de software interactivas de tiempo real</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,6 +473,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -497,7 +513,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="57">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -986,39 +1002,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -1034,19 +1052,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1080,17 +1085,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -1214,6 +1208,55 @@
         <color auto="1"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1223,7 +1266,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1248,9 +1291,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1278,22 +1318,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1305,7 +1339,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1318,31 +1352,245 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1350,19 +1598,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1374,224 +1610,59 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2013,8 +2084,8 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="30" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:A40"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="30" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2028,927 +2099,957 @@
     <col min="7" max="7" width="14.7265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.26953125" style="5" customWidth="1"/>
     <col min="9" max="9" width="11.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="30.26953125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="46.1796875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="25.81640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="23" style="1" customWidth="1"/>
+    <col min="10" max="10" width="30.26953125" style="123" customWidth="1"/>
+    <col min="11" max="11" width="46.1796875" style="117" customWidth="1"/>
+    <col min="12" max="12" width="25.81640625" style="128" customWidth="1"/>
+    <col min="13" max="13" width="23" style="123" customWidth="1"/>
     <col min="14" max="14" width="20.26953125" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="29.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="59"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="96"/>
     </row>
     <row r="2" spans="1:13" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="62"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="99"/>
     </row>
     <row r="3" spans="1:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="65"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="102"/>
     </row>
     <row r="4" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="69"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="106"/>
     </row>
     <row r="5" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="107" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="73"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="110"/>
     </row>
     <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="77"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="78"/>
     </row>
     <row r="7" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="78">
+      <c r="B7" s="79">
         <v>15016</v>
       </c>
-      <c r="C7" s="78"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="81"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="82"/>
     </row>
     <row r="8" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="89">
+      <c r="B8" s="65">
         <v>2</v>
       </c>
-      <c r="C8" s="90"/>
-      <c r="D8" s="27" t="s">
+      <c r="C8" s="66"/>
+      <c r="D8" s="24" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="9">
         <v>96</v>
       </c>
-      <c r="F8" s="94" t="s">
+      <c r="F8" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="94"/>
+      <c r="G8" s="93"/>
       <c r="H8" s="9">
         <v>64</v>
       </c>
-      <c r="I8" s="91" t="s">
+      <c r="I8" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="10">
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="129">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="85"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="85"/>
+      <c r="M9" s="86"/>
     </row>
     <row r="10" spans="1:13" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="87"/>
-      <c r="M10" s="88"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="88"/>
+      <c r="M10" s="89"/>
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="46" t="s">
+      <c r="E11" s="114"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="114"/>
+      <c r="H11" s="114"/>
+      <c r="I11" s="114"/>
+      <c r="J11" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="48" t="s">
+      <c r="K11" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="46" t="s">
+      <c r="L11" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="46" t="s">
+      <c r="M11" s="41" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="53"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="26" t="s">
+      <c r="A12" s="116"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="37" t="s">
+      <c r="I12" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="47"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-    </row>
-    <row r="13" spans="1:13" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="14" t="s">
+      <c r="J12" s="42"/>
+      <c r="K12" s="135"/>
+      <c r="L12" s="125"/>
+      <c r="M12" s="42"/>
+    </row>
+    <row r="13" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="116"/>
+      <c r="B13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" s="136" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="21" t="s">
+      <c r="L13" s="126" t="s">
         <v>63</v>
       </c>
-      <c r="K13" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L13" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="M13" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="M13" s="130">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="116"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="54" t="s">
-        <v>65</v>
+      <c r="C14" s="46" t="s">
+        <v>69</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H14" s="8"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K14" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L14" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="M14" s="42">
+      <c r="I14" s="18"/>
+      <c r="J14" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="L14" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="130">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+    <row r="15" spans="1:13" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="116"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="55"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H15" s="8"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K15" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L15" s="20" t="s">
+      <c r="I15" s="18"/>
+      <c r="J15" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="M15" s="42">
+      <c r="K15" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M15" s="130">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
+    <row r="16" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="116"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="55"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="H16" s="8"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K16" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L16" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="M16" s="42">
+      <c r="I16" s="18"/>
+      <c r="J16" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M16" s="130">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
+    <row r="17" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="116"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K17" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L17" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="M17" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="118" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17" s="137" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" s="127" t="s">
+        <v>63</v>
+      </c>
+      <c r="M17" s="131">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="116"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="56"/>
+      <c r="C18" s="46" t="s">
+        <v>75</v>
+      </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="18"/>
+      <c r="J18" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K18" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L18" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="M18" s="43">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
+      <c r="K18" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M18" s="130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="116"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="54" t="s">
-        <v>72</v>
-      </c>
+      <c r="C19" s="47"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H19" s="8"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K19" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L19" s="20" t="s">
+      <c r="I19" s="18"/>
+      <c r="J19" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="M19" s="42">
+      <c r="K19" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" s="130">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
+    <row r="20" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="116"/>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="55"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="H20" s="8"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K20" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L20" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="M20" s="42">
+      <c r="I20" s="18"/>
+      <c r="J20" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" s="130">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
+      <c r="A21" s="116"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K21" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L21" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="M21" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="21"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="118" t="s">
+        <v>73</v>
+      </c>
+      <c r="K21" s="137" t="s">
+        <v>61</v>
+      </c>
+      <c r="L21" s="127" t="s">
+        <v>63</v>
+      </c>
+      <c r="M21" s="131">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="70" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="116"/>
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="56"/>
+      <c r="C22" s="43" t="s">
+        <v>76</v>
+      </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H22" s="8"/>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="18"/>
+      <c r="J22" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K22" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L22" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="M22" s="43">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
+      <c r="K22" s="132" t="s">
+        <v>61</v>
+      </c>
+      <c r="L22" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M22" s="130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="116"/>
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="124" t="s">
-        <v>73</v>
-      </c>
+      <c r="C23" s="44"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H23" s="8"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K23" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L23" s="20" t="s">
+      <c r="I23" s="18"/>
+      <c r="J23" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="M23" s="42">
+      <c r="K23" s="132" t="s">
+        <v>61</v>
+      </c>
+      <c r="L23" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="130">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
+    <row r="24" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="116"/>
       <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="125"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="H24" s="8"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K24" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L24" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="M24" s="42">
+      <c r="I24" s="18"/>
+      <c r="J24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24" s="132" t="s">
+        <v>61</v>
+      </c>
+      <c r="L24" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M24" s="130">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
+      <c r="A25" s="116"/>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="126"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="19" t="s">
-        <v>67</v>
-      </c>
+      <c r="C25" s="45"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="I25" s="12"/>
       <c r="J25" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K25" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L25" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="M25" s="43">
+        <v>73</v>
+      </c>
+      <c r="K25" s="133" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" s="126" t="s">
+        <v>63</v>
+      </c>
+      <c r="M25" s="119">
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
+    <row r="26" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="116"/>
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="54" t="s">
-        <v>74</v>
+      <c r="C26" s="46" t="s">
+        <v>77</v>
       </c>
       <c r="D26" s="7"/>
-      <c r="E26" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="E26" s="30"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H26" s="8"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L26" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="M26" s="42">
+      <c r="I26" s="18"/>
+      <c r="J26" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="K26" s="132" t="s">
+        <v>61</v>
+      </c>
+      <c r="L26" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M26" s="130">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
+    <row r="27" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="116"/>
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="55"/>
+      <c r="C27" s="47"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H27" s="8"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L27" s="20" t="s">
+      <c r="I27" s="18"/>
+      <c r="J27" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="M27" s="42">
+      <c r="K27" s="132" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M27" s="130">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
+    <row r="28" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="116"/>
       <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="56"/>
+      <c r="C28" s="47"/>
       <c r="D28" s="7"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="H28" s="8"/>
-      <c r="I28" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L28" s="20" t="s">
+      <c r="I28" s="18"/>
+      <c r="J28" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="M28" s="43">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
+      <c r="K28" s="132" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="M28" s="130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+      <c r="A29" s="116"/>
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="21"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K29" s="133" t="s">
+        <v>61</v>
+      </c>
+      <c r="L29" s="126" t="s">
+        <v>63</v>
+      </c>
+      <c r="M29" s="119">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
+      <c r="A30" s="116"/>
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="39"/>
+      <c r="C30" s="33"/>
       <c r="D30" s="7"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="19"/>
+      <c r="I30" s="18"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
+      <c r="K30" s="134"/>
+      <c r="L30" s="126"/>
+      <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="53"/>
-      <c r="B31" s="22" t="s">
+      <c r="A31" s="116"/>
+      <c r="B31" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="138"/>
+      <c r="L31" s="127"/>
+      <c r="M31" s="22"/>
     </row>
     <row r="32" spans="1:13" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="105" t="s">
+      <c r="B32" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="106"/>
-      <c r="D32" s="106"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="106"/>
-      <c r="H32" s="107"/>
-      <c r="I32" s="36" t="s">
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="J32" s="101" t="s">
+      <c r="J32" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="K32" s="102"/>
-      <c r="L32" s="102"/>
-      <c r="M32" s="103"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="54"/>
     </row>
     <row r="33" spans="1:13" ht="55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="104"/>
-      <c r="B33" s="108" t="s">
+      <c r="A33" s="55"/>
+      <c r="B33" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="109"/>
-      <c r="D33" s="109"/>
-      <c r="E33" s="109"/>
-      <c r="F33" s="109"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="110"/>
-      <c r="I33" s="35" t="s">
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="120" t="s">
         <v>55</v>
       </c>
-      <c r="J33" s="116" t="s">
+      <c r="J33" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="K33" s="117"/>
-      <c r="L33" s="117"/>
-      <c r="M33" s="118"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="71"/>
     </row>
     <row r="34" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="104"/>
-      <c r="B34" s="111" t="s">
+      <c r="A34" s="55"/>
+      <c r="B34" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="112"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="112"/>
-      <c r="H34" s="113"/>
-      <c r="I34" s="33" t="s">
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="121" t="s">
         <v>55</v>
       </c>
-      <c r="J34" s="119" t="s">
+      <c r="J34" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="K34" s="120"/>
-      <c r="L34" s="120"/>
-      <c r="M34" s="121"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="74"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="104"/>
-      <c r="B35" s="89"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="90"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="95"/>
-      <c r="K35" s="96"/>
-      <c r="L35" s="96"/>
-      <c r="M35" s="97"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="121"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="38"/>
     </row>
     <row r="36" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="104"/>
-      <c r="B36" s="89"/>
-      <c r="C36" s="96"/>
-      <c r="D36" s="96"/>
-      <c r="E36" s="96"/>
-      <c r="F36" s="96"/>
-      <c r="G36" s="96"/>
-      <c r="H36" s="90"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="95"/>
-      <c r="K36" s="96"/>
-      <c r="L36" s="96"/>
-      <c r="M36" s="97"/>
+      <c r="A36" s="55"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="121"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="38"/>
     </row>
     <row r="37" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="104"/>
-      <c r="B37" s="89"/>
-      <c r="C37" s="96"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="96"/>
-      <c r="F37" s="96"/>
-      <c r="G37" s="96"/>
-      <c r="H37" s="90"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="95"/>
-      <c r="K37" s="96"/>
-      <c r="L37" s="96"/>
-      <c r="M37" s="97"/>
+      <c r="A37" s="55"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="121"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="38"/>
     </row>
     <row r="38" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="104"/>
-      <c r="B38" s="89"/>
-      <c r="C38" s="96"/>
-      <c r="D38" s="96"/>
-      <c r="E38" s="96"/>
-      <c r="F38" s="96"/>
-      <c r="G38" s="96"/>
-      <c r="H38" s="90"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="95"/>
-      <c r="K38" s="96"/>
-      <c r="L38" s="96"/>
-      <c r="M38" s="97"/>
+      <c r="A38" s="55"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="121"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="38"/>
     </row>
     <row r="39" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="104"/>
-      <c r="B39" s="89"/>
-      <c r="C39" s="96"/>
-      <c r="D39" s="96"/>
-      <c r="E39" s="96"/>
-      <c r="F39" s="96"/>
-      <c r="G39" s="96"/>
-      <c r="H39" s="90"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="96"/>
-      <c r="L39" s="96"/>
-      <c r="M39" s="97"/>
+      <c r="A39" s="55"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="121"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="38"/>
     </row>
     <row r="40" spans="1:13" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="47"/>
-      <c r="B40" s="114"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="99"/>
-      <c r="F40" s="99"/>
-      <c r="G40" s="99"/>
-      <c r="H40" s="115"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="98"/>
-      <c r="K40" s="99"/>
-      <c r="L40" s="99"/>
-      <c r="M40" s="100"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="122"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="50"/>
+      <c r="L40" s="50"/>
+      <c r="M40" s="51"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="A13:C31 I12 I11:J11 L11 A11:C11 K11:K12 I29:M31 I14:I17 I13:M13 I19:I21 I23:I24 K14:M25 D11:H31 I26:I27 J26:M28" name="Rango1"/>
-    <protectedRange sqref="I18:J18 I22:J22 I25:J25 I28" name="Rango1_1"/>
-    <protectedRange sqref="J14:J17 J19:J21 J23:J24" name="Rango1_3"/>
+    <protectedRange sqref="I12 I11:J11 L11 A11:C11 D11:H12 A13:B13 K11:K13 A14:D17 E15:E17 G14:I16 A19:B31 D30:M31 A18:C18 E19:E21 G18:I20 C20:C22 C24:C31 E23:E25 G22:I24 K14:M29 D18:D29 F14:F29 E27:E29 G26:I28" name="Rango1"/>
+    <protectedRange sqref="J14:J16 J18:J20 J22:J24 J26:J28" name="Rango1_3"/>
+    <protectedRange sqref="C13:J13 L13:M13" name="Rango1_2"/>
+    <protectedRange sqref="G17:H17 J17 G21:H21 J21 G25:H25 J25 G29:H29 J29" name="Rango1_4"/>
+    <protectedRange sqref="I17 I21 I25 I29" name="Rango1_1_1"/>
   </protectedRanges>
   <mergeCells count="43">
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="A11:A31"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="D10:M10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="J38:M38"/>
     <mergeCell ref="J39:M39"/>
     <mergeCell ref="J40:M40"/>
@@ -2965,25 +3066,12 @@
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="J33:M33"/>
     <mergeCell ref="J34:M34"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="D10:M10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="A11:A31"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:C10" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2995,22 +3083,46 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B34" r:id="rId1" display="https://sistemascomputacionales.readthedocs.io/es/v2022.20" xr:uid="{F483E0E0-E4A7-4C2F-860A-EBA3E7D139F7}"/>
-    <hyperlink ref="K13" r:id="rId2" xr:uid="{D6255421-56CE-4DA6-B03E-76DEDA9FDF65}"/>
-    <hyperlink ref="K14:K28" r:id="rId3" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{110D775A-2750-4A7D-B2A4-BA2561889554}"/>
-    <hyperlink ref="K19:K22" r:id="rId4" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{0DB1E3FF-C0FB-46C2-8DED-ECA63BDF07D8}"/>
-    <hyperlink ref="K23:K25" r:id="rId5" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{E87DE1B2-50DB-4A33-8393-C7703364CEAE}"/>
+    <hyperlink ref="K14:K28" r:id="rId2" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{110D775A-2750-4A7D-B2A4-BA2561889554}"/>
+    <hyperlink ref="K19:K22" r:id="rId3" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{0DB1E3FF-C0FB-46C2-8DED-ECA63BDF07D8}"/>
+    <hyperlink ref="K13" r:id="rId4" xr:uid="{E9C4F801-5F86-40D4-BD31-1C88E427E0B0}"/>
+    <hyperlink ref="K18:K21" r:id="rId5" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{E4A0F34D-882D-4E3A-AB67-D4DCE09FF653}"/>
+    <hyperlink ref="K22:K25" r:id="rId6" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{E2559DF7-D3EE-436E-9373-897FB822BB8D}"/>
+    <hyperlink ref="K23:K25" r:id="rId7" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{332153DD-F144-4DAC-842B-E91AE2F93E03}"/>
+    <hyperlink ref="K26:K29" r:id="rId8" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{067FFFDF-B543-4F2C-B40B-402A53BD76CF}"/>
+    <hyperlink ref="K26" r:id="rId9" xr:uid="{2B2C0214-6EBF-4B2A-AFDA-EC7956C55FB6}"/>
+    <hyperlink ref="K27:K29" r:id="rId10" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{F56A05E5-B7BF-452B-B0AC-92BAAA1443C7}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.2736614173228347" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId6"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId11"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="13" max="53" man="1"/>
   </colBreaks>
-  <legacyDrawing r:id="rId7"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="475903d6-5b88-4d7a-ba78-d123e191ef42" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007385DC504DB614DA8F67D4315A28B14" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ac3543c8bd13c0fc9dcbaaaa4f4e21f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="1be38a3c-13c4-46e0-8a29-91f320e906cc" xmlns:ns4="475903d6-5b88-4d7a-ba78-d123e191ef42" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="832580f857820fba5b25e66e4b08a8f5" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3268,26 +3380,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDE66BE-7C4D-4D57-9569-773F449FD84D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1be38a3c-13c4-46e0-8a29-91f320e906cc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="475903d6-5b88-4d7a-ba78-d123e191ef42"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_activity xmlns="475903d6-5b88-4d7a-ba78-d123e191ef42" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635976DF-2941-4508-B3B6-F1CF25643BD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C325370-FB0B-42DC-B685-563E2C80434A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3305,30 +3424,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635976DF-2941-4508-B3B6-F1CF25643BD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDE66BE-7C4D-4D57-9569-773F449FD84D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1be38a3c-13c4-46e0-8a29-91f320e906cc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="475903d6-5b88-4d7a-ba78-d123e191ef42"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update proyecto docente and intro
</commit_message>
<xml_diff>
--- a/docs/_static/FormatoPlaneacionInteractivos12023-10.xlsx
+++ b/docs/_static/FormatoPlaneacionInteractivos12023-10.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76988EA2-D9F0-464B-B1D6-481B7BCAB805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15777194-A852-42B3-9B2F-076C2C340176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,21 @@
     <definedName name="AMPLIONBC">[1]Listas!$H$2:$H$11</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Proyecto Docente'!$A$1:$M$31</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -109,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="78">
   <si>
     <t>PROYECTO DOCENTE</t>
   </si>
@@ -378,7 +389,7 @@
     <t>Unidad 3: protocolos binarios</t>
   </si>
   <si>
-    <t>Unidad 4: plataformas de software interactivas de tiempo real</t>
+    <t>Unidad 4: proyecto</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1277,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1367,250 +1378,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1621,12 +1388,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1652,9 +1413,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1663,6 +1421,258 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2084,8 +2094,8 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="30" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="30" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2099,169 +2109,169 @@
     <col min="7" max="7" width="14.7265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.26953125" style="5" customWidth="1"/>
     <col min="9" max="9" width="11.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="30.26953125" style="123" customWidth="1"/>
-    <col min="11" max="11" width="46.1796875" style="117" customWidth="1"/>
-    <col min="12" max="12" width="25.81640625" style="128" customWidth="1"/>
-    <col min="13" max="13" width="23" style="123" customWidth="1"/>
+    <col min="10" max="10" width="30.26953125" style="41" customWidth="1"/>
+    <col min="11" max="11" width="46.1796875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="25.81640625" style="44" customWidth="1"/>
+    <col min="13" max="13" width="23" style="41" customWidth="1"/>
     <col min="14" max="14" width="20.26953125" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="29.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="96"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="71"/>
     </row>
     <row r="2" spans="1:13" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="99"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
     </row>
     <row r="3" spans="1:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="102"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
     </row>
     <row r="4" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="103"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="106"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="81"/>
     </row>
     <row r="5" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="109"/>
-      <c r="M5" s="110"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="85"/>
     </row>
     <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="78"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="89"/>
     </row>
     <row r="7" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="79">
+      <c r="B7" s="90">
         <v>15016</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="82"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="93"/>
     </row>
     <row r="8" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="65">
+      <c r="B8" s="101">
         <v>2</v>
       </c>
-      <c r="C8" s="66"/>
+      <c r="C8" s="102"/>
       <c r="D8" s="24" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="9">
         <v>96</v>
       </c>
-      <c r="F8" s="93" t="s">
+      <c r="F8" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="93"/>
+      <c r="G8" s="106"/>
       <c r="H8" s="9">
         <v>64</v>
       </c>
-      <c r="I8" s="90" t="s">
+      <c r="I8" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="129">
+      <c r="J8" s="104"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="45">
         <v>32</v>
       </c>
     </row>
@@ -2269,20 +2279,20 @@
       <c r="A9" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="86"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="95"/>
+      <c r="H9" s="95"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="95"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="97"/>
     </row>
     <row r="10" spans="1:13" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
@@ -2292,52 +2302,52 @@
         <v>43</v>
       </c>
       <c r="C10" s="25"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="87"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="89"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="99"/>
+      <c r="M10" s="100"/>
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="115" t="s">
+      <c r="A11" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="111" t="s">
+      <c r="B11" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="113" t="s">
+      <c r="D11" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
-      <c r="G11" s="114"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="114"/>
-      <c r="J11" s="41" t="s">
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="114" t="s">
+      <c r="K11" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="124" t="s">
+      <c r="L11" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="41" t="s">
+      <c r="M11" s="56" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="116"/>
-      <c r="B12" s="112"/>
-      <c r="C12" s="40"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="135"/>
       <c r="D12" s="23" t="s">
         <v>5</v>
       </c>
@@ -2356,13 +2366,13 @@
       <c r="I12" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="42"/>
-      <c r="K12" s="135"/>
-      <c r="L12" s="125"/>
-      <c r="M12" s="42"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="137"/>
+      <c r="M12" s="57"/>
     </row>
     <row r="13" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="116"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="13" t="s">
         <v>41</v>
       </c>
@@ -2382,22 +2392,22 @@
       <c r="J13" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="136" t="s">
+      <c r="K13" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="L13" s="126" t="s">
+      <c r="L13" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="M13" s="130">
+      <c r="M13" s="46">
         <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="116"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="63" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="7"/>
@@ -2410,22 +2420,22 @@
       <c r="J14" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="136" t="s">
+      <c r="K14" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="L14" s="126" t="s">
+      <c r="L14" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M14" s="130">
+      <c r="M14" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="116"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="64"/>
       <c r="D15" s="7"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -2437,22 +2447,22 @@
       <c r="J15" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="K15" s="136" t="s">
+      <c r="K15" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="L15" s="126" t="s">
+      <c r="L15" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M15" s="130">
+      <c r="M15" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="116"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="47"/>
+      <c r="C16" s="64"/>
       <c r="D16" s="7"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -2464,22 +2474,22 @@
       <c r="J16" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="K16" s="136" t="s">
+      <c r="K16" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="L16" s="126" t="s">
+      <c r="L16" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M16" s="130">
+      <c r="M16" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="116"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="47"/>
+      <c r="C17" s="64"/>
       <c r="D17" s="10"/>
       <c r="E17" s="4"/>
       <c r="F17" s="11"/>
@@ -2488,25 +2498,25 @@
       </c>
       <c r="H17" s="21"/>
       <c r="I17" s="12"/>
-      <c r="J17" s="118" t="s">
+      <c r="J17" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="K17" s="137" t="s">
+      <c r="K17" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="L17" s="127" t="s">
+      <c r="L17" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="M17" s="131">
+      <c r="M17" s="47">
         <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="116"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="63" t="s">
         <v>75</v>
       </c>
       <c r="D18" s="7"/>
@@ -2520,22 +2530,22 @@
       <c r="J18" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="K18" s="136" t="s">
+      <c r="K18" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="L18" s="126" t="s">
+      <c r="L18" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M18" s="130">
+      <c r="M18" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="116"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="47"/>
+      <c r="C19" s="64"/>
       <c r="D19" s="7"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -2547,22 +2557,22 @@
       <c r="J19" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="K19" s="136" t="s">
+      <c r="K19" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="126" t="s">
+      <c r="L19" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M19" s="130">
+      <c r="M19" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="116"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="47"/>
+      <c r="C20" s="64"/>
       <c r="D20" s="7"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -2574,22 +2584,22 @@
       <c r="J20" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="K20" s="136" t="s">
+      <c r="K20" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="L20" s="126" t="s">
+      <c r="L20" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M20" s="130">
+      <c r="M20" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A21" s="116"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="48"/>
+      <c r="C21" s="65"/>
       <c r="D21" s="10"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -2598,25 +2608,25 @@
       </c>
       <c r="H21" s="21"/>
       <c r="I21" s="12"/>
-      <c r="J21" s="118" t="s">
+      <c r="J21" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="K21" s="137" t="s">
+      <c r="K21" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="L21" s="127" t="s">
+      <c r="L21" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="M21" s="131">
+      <c r="M21" s="47">
         <v>0.25</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="70" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="116"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="66" t="s">
         <v>76</v>
       </c>
       <c r="D22" s="7"/>
@@ -2630,22 +2640,22 @@
       <c r="J22" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="132" t="s">
+      <c r="K22" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="L22" s="126" t="s">
+      <c r="L22" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M22" s="130">
+      <c r="M22" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="116"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="44"/>
+      <c r="C23" s="67"/>
       <c r="D23" s="7"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -2657,22 +2667,22 @@
       <c r="J23" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="K23" s="132" t="s">
+      <c r="K23" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="L23" s="126" t="s">
+      <c r="L23" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M23" s="130">
+      <c r="M23" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="116"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="44"/>
+      <c r="C24" s="67"/>
       <c r="D24" s="7"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -2684,22 +2694,22 @@
       <c r="J24" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="K24" s="132" t="s">
+      <c r="K24" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="L24" s="126" t="s">
+      <c r="L24" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M24" s="130">
+      <c r="M24" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A25" s="116"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="45"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="10"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
@@ -2711,22 +2721,22 @@
       <c r="J25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K25" s="133" t="s">
+      <c r="K25" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="L25" s="126" t="s">
+      <c r="L25" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="M25" s="119">
+      <c r="M25" s="37">
         <v>0.25</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="116"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="63" t="s">
         <v>77</v>
       </c>
       <c r="D26" s="7"/>
@@ -2740,22 +2750,22 @@
       <c r="J26" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="K26" s="132" t="s">
+      <c r="K26" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="L26" s="126" t="s">
+      <c r="L26" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M26" s="130">
+      <c r="M26" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="116"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="47"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="7"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -2767,72 +2777,65 @@
       <c r="J27" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="K27" s="132" t="s">
+      <c r="K27" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="L27" s="126" t="s">
+      <c r="L27" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="M27" s="130">
+      <c r="M27" s="46">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="116"/>
+    <row r="28" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+      <c r="A28" s="62"/>
       <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="47"/>
+      <c r="C28" s="64"/>
       <c r="D28" s="7"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="18"/>
+      <c r="G28" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" s="21"/>
+      <c r="I28" s="12"/>
       <c r="J28" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K28" s="132" t="s">
+        <v>73</v>
+      </c>
+      <c r="K28" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="L28" s="126" t="s">
-        <v>62</v>
-      </c>
-      <c r="M28" s="130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A29" s="116"/>
+      <c r="L28" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M28" s="37">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="62"/>
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H29" s="21"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K29" s="133" t="s">
-        <v>61</v>
-      </c>
-      <c r="L29" s="126" t="s">
-        <v>63</v>
-      </c>
-      <c r="M29" s="119">
-        <v>0.25</v>
+      <c r="C29" s="15"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="37">
+        <f>SUM(M12:M28)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="116"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
@@ -2844,12 +2847,12 @@
       <c r="H30" s="8"/>
       <c r="I30" s="18"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="134"/>
-      <c r="L30" s="126"/>
-      <c r="M30" s="3"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="37"/>
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="116"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="20" t="s">
         <v>29</v>
       </c>
@@ -2861,195 +2864,181 @@
       <c r="H31" s="21"/>
       <c r="I31" s="12"/>
       <c r="J31" s="22"/>
-      <c r="K31" s="138"/>
-      <c r="L31" s="127"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="43"/>
       <c r="M31" s="22"/>
     </row>
     <row r="32" spans="1:13" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="58"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="119"/>
       <c r="I32" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="J32" s="52" t="s">
+      <c r="J32" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="54"/>
+      <c r="K32" s="114"/>
+      <c r="L32" s="114"/>
+      <c r="M32" s="115"/>
     </row>
     <row r="33" spans="1:13" ht="55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="55"/>
-      <c r="B33" s="59" t="s">
+      <c r="A33" s="116"/>
+      <c r="B33" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="120" t="s">
+      <c r="C33" s="121"/>
+      <c r="D33" s="121"/>
+      <c r="E33" s="121"/>
+      <c r="F33" s="121"/>
+      <c r="G33" s="121"/>
+      <c r="H33" s="122"/>
+      <c r="I33" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="J33" s="69" t="s">
+      <c r="J33" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="K33" s="70"/>
-      <c r="L33" s="70"/>
-      <c r="M33" s="71"/>
+      <c r="K33" s="129"/>
+      <c r="L33" s="129"/>
+      <c r="M33" s="130"/>
     </row>
     <row r="34" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="55"/>
-      <c r="B34" s="62" t="s">
+      <c r="A34" s="116"/>
+      <c r="B34" s="123" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="121" t="s">
+      <c r="C34" s="124"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="124"/>
+      <c r="H34" s="125"/>
+      <c r="I34" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="J34" s="72" t="s">
+      <c r="J34" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="K34" s="73"/>
-      <c r="L34" s="73"/>
-      <c r="M34" s="74"/>
+      <c r="K34" s="132"/>
+      <c r="L34" s="132"/>
+      <c r="M34" s="133"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
-      <c r="B35" s="65"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="121"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="38"/>
+      <c r="A35" s="116"/>
+      <c r="B35" s="101"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="108"/>
+      <c r="F35" s="108"/>
+      <c r="G35" s="108"/>
+      <c r="H35" s="102"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="107"/>
+      <c r="K35" s="108"/>
+      <c r="L35" s="108"/>
+      <c r="M35" s="109"/>
     </row>
     <row r="36" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="55"/>
-      <c r="B36" s="65"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="121"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="38"/>
+      <c r="A36" s="116"/>
+      <c r="B36" s="101"/>
+      <c r="C36" s="108"/>
+      <c r="D36" s="108"/>
+      <c r="E36" s="108"/>
+      <c r="F36" s="108"/>
+      <c r="G36" s="108"/>
+      <c r="H36" s="102"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="107"/>
+      <c r="K36" s="108"/>
+      <c r="L36" s="108"/>
+      <c r="M36" s="109"/>
     </row>
     <row r="37" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="55"/>
-      <c r="B37" s="65"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="121"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="38"/>
+      <c r="A37" s="116"/>
+      <c r="B37" s="101"/>
+      <c r="C37" s="108"/>
+      <c r="D37" s="108"/>
+      <c r="E37" s="108"/>
+      <c r="F37" s="108"/>
+      <c r="G37" s="108"/>
+      <c r="H37" s="102"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="107"/>
+      <c r="K37" s="108"/>
+      <c r="L37" s="108"/>
+      <c r="M37" s="109"/>
     </row>
     <row r="38" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="55"/>
-      <c r="B38" s="65"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="66"/>
-      <c r="I38" s="121"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="38"/>
+      <c r="A38" s="116"/>
+      <c r="B38" s="101"/>
+      <c r="C38" s="108"/>
+      <c r="D38" s="108"/>
+      <c r="E38" s="108"/>
+      <c r="F38" s="108"/>
+      <c r="G38" s="108"/>
+      <c r="H38" s="102"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="107"/>
+      <c r="K38" s="108"/>
+      <c r="L38" s="108"/>
+      <c r="M38" s="109"/>
     </row>
     <row r="39" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="55"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="66"/>
-      <c r="I39" s="121"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="38"/>
+      <c r="A39" s="116"/>
+      <c r="B39" s="101"/>
+      <c r="C39" s="108"/>
+      <c r="D39" s="108"/>
+      <c r="E39" s="108"/>
+      <c r="F39" s="108"/>
+      <c r="G39" s="108"/>
+      <c r="H39" s="102"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="107"/>
+      <c r="K39" s="108"/>
+      <c r="L39" s="108"/>
+      <c r="M39" s="109"/>
     </row>
     <row r="40" spans="1:13" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="42"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="122"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="50"/>
-      <c r="L40" s="50"/>
-      <c r="M40" s="51"/>
+      <c r="A40" s="57"/>
+      <c r="B40" s="126"/>
+      <c r="C40" s="111"/>
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
+      <c r="F40" s="111"/>
+      <c r="G40" s="111"/>
+      <c r="H40" s="127"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="110"/>
+      <c r="K40" s="111"/>
+      <c r="L40" s="111"/>
+      <c r="M40" s="112"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="I12 I11:J11 L11 A11:C11 D11:H12 A13:B13 K11:K13 A14:D17 E15:E17 G14:I16 A19:B31 D30:M31 A18:C18 E19:E21 G18:I20 C20:C22 C24:C31 E23:E25 G22:I24 K14:M29 D18:D29 F14:F29 E27:E29 G26:I28" name="Rango1"/>
-    <protectedRange sqref="J14:J16 J18:J20 J22:J24 J26:J28" name="Rango1_3"/>
+    <protectedRange sqref="I12 I11:J11 L11 A11:C11 D11:H12 A13:B13 K11:K13 A14:D17 E15:E17 G14:I16 A19:B31 A18:C18 E19:E21 G18:I20 C20:C22 C24:C31 E23:E25 G22:I24 D18:D28 F14:F28 E27:E28 G26:I27 K14:M28 D29:M31" name="Rango1"/>
+    <protectedRange sqref="J14:J16 J18:J20 J22:J24 J26:J27" name="Rango1_3"/>
     <protectedRange sqref="C13:J13 L13:M13" name="Rango1_2"/>
-    <protectedRange sqref="G17:H17 J17 G21:H21 J21 G25:H25 J25 G29:H29 J29" name="Rango1_4"/>
-    <protectedRange sqref="I17 I21 I25 I29" name="Rango1_1_1"/>
+    <protectedRange sqref="G17:H17 J17 G21:H21 J21 G25:H25 J25 G28:H28 J28" name="Rango1_4"/>
+    <protectedRange sqref="I17 I21 I25 I28" name="Rango1_1_1"/>
   </protectedRanges>
   <mergeCells count="43">
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="A11:A31"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="D10:M10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="C26:C28"/>
     <mergeCell ref="J38:M38"/>
     <mergeCell ref="J39:M39"/>
     <mergeCell ref="J40:M40"/>
@@ -3066,12 +3055,26 @@
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="J33:M33"/>
     <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="D10:M10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="A11:A31"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="C22:C25"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:C10" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -3089,9 +3092,9 @@
     <hyperlink ref="K18:K21" r:id="rId5" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{E4A0F34D-882D-4E3A-AB67-D4DCE09FF653}"/>
     <hyperlink ref="K22:K25" r:id="rId6" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{E2559DF7-D3EE-436E-9373-897FB822BB8D}"/>
     <hyperlink ref="K23:K25" r:id="rId7" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{332153DD-F144-4DAC-842B-E91AE2F93E03}"/>
-    <hyperlink ref="K26:K29" r:id="rId8" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{067FFFDF-B543-4F2C-B40B-402A53BD76CF}"/>
+    <hyperlink ref="K26:K28" r:id="rId8" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{067FFFDF-B543-4F2C-B40B-402A53BD76CF}"/>
     <hyperlink ref="K26" r:id="rId9" xr:uid="{2B2C0214-6EBF-4B2A-AFDA-EC7956C55FB6}"/>
-    <hyperlink ref="K27:K29" r:id="rId10" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{F56A05E5-B7BF-452B-B0AC-92BAAA1443C7}"/>
+    <hyperlink ref="K27:K28" r:id="rId10" display="https://sistemasfisicosinteractivos1.readthedocs.io/" xr:uid="{F56A05E5-B7BF-452B-B0AC-92BAAA1443C7}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.2736614173228347" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3104,25 +3107,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_activity xmlns="475903d6-5b88-4d7a-ba78-d123e191ef42" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007385DC504DB614DA8F67D4315A28B14" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ac3543c8bd13c0fc9dcbaaaa4f4e21f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="1be38a3c-13c4-46e0-8a29-91f320e906cc" xmlns:ns4="475903d6-5b88-4d7a-ba78-d123e191ef42" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="832580f857820fba5b25e66e4b08a8f5" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3380,33 +3364,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDE66BE-7C4D-4D57-9569-773F449FD84D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1be38a3c-13c4-46e0-8a29-91f320e906cc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="475903d6-5b88-4d7a-ba78-d123e191ef42"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635976DF-2941-4508-B3B6-F1CF25643BD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="475903d6-5b88-4d7a-ba78-d123e191ef42" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C325370-FB0B-42DC-B685-563E2C80434A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3424,4 +3401,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635976DF-2941-4508-B3B6-F1CF25643BD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDE66BE-7C4D-4D57-9569-773F449FD84D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1be38a3c-13c4-46e0-8a29-91f320e906cc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="475903d6-5b88-4d7a-ba78-d123e191ef42"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>